<commit_message>
Integrate csv conversions (#12)
* Added a properties file for colours so they are not hard-coded into main.py

* Added a properties file for colours so they are not hard-coded into main.py

* Added a properties file for colours so they are not hard-coded into main.py

* Updated comments

* new file

* debug only

* Added a properties file for colours so they are not hard-coded into main.py

* Added Test case and renamed main.py

* Added some file checks

* Added some file checks

* Added some file checks

* Conversion from csv to excel

* Improve tests for conversions

* Improve tests for conversions

* Integrate csv to xlsx conversion in code

* Added simple TODO

* Added README until I can merge it to main README
</commit_message>
<xml_diff>
--- a/Users.xlsx
+++ b/Users.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11127"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petercaron/PycharmProjects/pythonPolarArea/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/petercaron/Downloads/git_repos/pythonPolarArea/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B03961F2-C02C-C447-86B9-14FAD0524941}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0896DA82-8FA1-C94D-A579-350B14D164EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9260" yWindow="1180" windowWidth="24960" windowHeight="16760" xr2:uid="{BF4DD9D4-7FFE-F041-8824-A4860B29AB1D}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16940" xr2:uid="{48724B4C-CE40-E044-8DBA-FDFD3866AFC3}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Peter" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="form_data__3" localSheetId="0">Sheet1!$A$1:$B$20</definedName>
+    <definedName name="Users_1" localSheetId="0">Peter!#REF!</definedName>
+    <definedName name="Users_2" localSheetId="0">Peter!$A$2:$S$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -29,9 +30,6 @@
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -40,9 +38,26 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{359824B3-0DD1-0D44-AD36-4C95FCCB2AC4}" name="form_data (3)" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/petercaron/Downloads/form_data (3).csv" decimal="," thousands="." comma="1">
-      <textFields count="2">
+  <connection id="1" xr16:uid="{DD0DA2C8-484B-B040-836C-7E4DEC047F5A}" name="Users1" type="6" refreshedVersion="6" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/petercaron/Downloads/git_repos/pythonPolarArea/Users.csv" decimal="," thousands="." tab="0" comma="1">
+      <textFields count="19">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
         <textField/>
         <textField/>
       </textFields>
@@ -54,67 +69,67 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
+    <t>Shared Vision</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Strategy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Business Alignment</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Subordinates for Success</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Cross-functional teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Clarity on priorities</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Acceptance Criteria</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enable Focus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Engagement</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Feedback</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Enable Autonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Change and ambiguity</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Desired Culture</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Work autonomously</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Stakeholders</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Customer Focus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Attrition</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Teams</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Develop People</t>
+  </si>
+  <si>
+    <t>Ratings</t>
+  </si>
+  <si>
     <t>Categories</t>
-  </si>
-  <si>
-    <t>Shared Vision</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Strategy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Business Alignment</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Subordinates for Success</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Cross-functional teams</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Clarity on priorities</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Acceptance Criteria</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enable Focus</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Engagement</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Feedback</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Enable Autonomy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Change and ambiguity</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Desired Culture</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Work autonomously</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Stakeholders</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Customer Focus</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Attrition</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Teams</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Develop People</t>
-  </si>
-  <si>
-    <t>Ratings</t>
   </si>
 </sst>
 </file>
@@ -125,7 +140,7 @@
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -170,7 +185,7 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="form_data (3)" connectionId="1" xr16:uid="{E71EEB1E-E455-6043-A0B6-398E9DCA0A86}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Users_2" connectionId="1" xr16:uid="{EB86E915-7CBA-E54F-9C03-77734785FC4D}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -184,39 +199,39 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="0E2841"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E8E8E8"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="156082"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="E97132"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="196B24"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="0F9ED5"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="A02B93"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="4EA72E"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="467886"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="96607D"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -268,7 +283,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -379,6 +394,13 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
         <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
@@ -387,13 +409,6 @@
           <a:miter lim="800000"/>
         </a:ln>
         <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -458,61 +473,73 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
+  <a:objectDefaults/>
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{961BC6E7-D84E-6641-B297-652649A53C4E}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FF0026B-890B-9D41-8932-67CE2A59A60A}">
   <dimension ref="A1:B20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="B2" sqref="B2:B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.5" customWidth="1"/>
+    <col min="3" max="3" width="19" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="21" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="7.83203125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="8" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="6.83203125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="33" max="34" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="7.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -520,55 +547,55 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3">
         <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4">
         <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5">
         <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6">
         <v>5</v>
-      </c>
-      <c r="B6">
-        <v>2</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9">
         <v>2</v>
@@ -576,31 +603,31 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13">
         <v>4</v>
@@ -608,15 +635,15 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>4</v>
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15">
         <v>4</v>
@@ -624,7 +651,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16">
         <v>3</v>
@@ -632,31 +659,31 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20">
         <v>3</v>

</xml_diff>